<commit_message>
07 atalhos excel fim
</commit_message>
<xml_diff>
--- a/004-atalhos/Atalhos-Use_Atalhos-Pasta_de_Trabalho1.xlsx
+++ b/004-atalhos/Atalhos-Use_Atalhos-Pasta_de_Trabalho1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jorge\Desktop\hashtag\hashtagExcel\004-atalhos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8388C32-2761-4B4F-B1EB-F88F984EB188}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B7467B3-5D6E-4389-993E-D25A0A76CFB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="978" activeTab="6" xr2:uid="{100ED8EA-C2B6-46A4-AE4B-962ED0DA143E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="978" activeTab="7" xr2:uid="{100ED8EA-C2B6-46A4-AE4B-962ED0DA143E}"/>
   </bookViews>
   <sheets>
     <sheet name="Ctrl T" sheetId="16" r:id="rId1"/>
@@ -284,10 +284,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="&quot;R$&quot;\ #,##0"/>
+    <numFmt numFmtId="166" formatCode="&quot;R$&quot;\ #,##0.00"/>
+    <numFmt numFmtId="167" formatCode="000&quot;.&quot;000&quot;.&quot;000&quot;-&quot;00"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -316,6 +318,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Abadi Extra Light"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="11">
@@ -407,7 +415,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -479,6 +487,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1540,8 +1560,8 @@
       <xdr:row>14</xdr:row>
       <xdr:rowOff>25400</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" Requires="sle15">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
+      <mc:Choice Requires="sle15">
         <xdr:graphicFrame macro="">
           <xdr:nvGraphicFramePr>
             <xdr:cNvPr id="2" name="Vendedor">
@@ -1564,7 +1584,7 @@
           </a:graphic>
         </xdr:graphicFrame>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="0" name=""/>
@@ -16724,7 +16744,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4830405-22B8-45A8-9799-C290B10CAADD}">
   <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
@@ -16941,13 +16961,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{134C23FC-40DE-4F9D-B1E5-CA571A968264}">
   <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="4" width="19.7109375" customWidth="1"/>
-    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="4" width="19.7109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="12.85546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="13.5703125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" style="1"/>
+    <col min="8" max="8" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -16965,228 +16990,237 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="29" t="s">
         <v>52</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="30">
         <v>10000</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="31">
         <v>44101</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="32">
         <v>56285537627</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="29" t="s">
         <v>53</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="30">
         <v>3200</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="31">
         <v>44170</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="32">
         <v>58866419137</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="29" t="s">
         <v>54</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="30">
         <v>7500</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="31">
         <v>43767</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="32">
         <v>79179596425</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="29" t="s">
         <v>55</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="30">
         <v>10000</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="31">
         <v>44026</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="32">
         <v>95288512163</v>
       </c>
+      <c r="F5" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="29" t="s">
         <v>56</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="30">
         <v>3200</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="31">
         <v>43471</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="32">
         <v>57181726328</v>
       </c>
+      <c r="F6" s="3">
+        <v>2</v>
+      </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="29" t="s">
         <v>57</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="30">
         <v>10000</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="31">
         <v>43630</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="32">
         <v>11247295455</v>
       </c>
+      <c r="F7" s="3">
+        <v>3</v>
+      </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="29" t="s">
         <v>58</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="30">
         <v>3200</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="31">
         <v>44192</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="32">
         <v>47111914389</v>
       </c>
-      <c r="H8" s="8"/>
+      <c r="H8" s="3"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="29" t="s">
         <v>59</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="30">
         <v>7500</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="31">
         <v>43639</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="32">
         <v>11814954552</v>
       </c>
-      <c r="H9" s="8"/>
+      <c r="H9" s="3"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="29" t="s">
         <v>60</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="30">
         <v>3200</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="31">
         <v>43744</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="32">
         <v>62611154618</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+      <c r="A11" s="29" t="s">
         <v>61</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="30">
         <v>10000</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="31">
         <v>43953</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="32">
         <v>57623538585</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+      <c r="A12" s="29" t="s">
         <v>62</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="30">
         <v>10000</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="31">
         <v>43665</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="32">
         <v>79936918176</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
+      <c r="A13" s="29" t="s">
         <v>63</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="30">
         <v>3200</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="31">
         <v>43434</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="32">
         <v>46917625558</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
+      <c r="A14" s="29" t="s">
         <v>64</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="30">
         <v>7500</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="31">
         <v>43783</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="32">
         <v>26517877354</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
+      <c r="A15" s="29" t="s">
         <v>65</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="30">
         <v>7500</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="31">
         <v>43784</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="32">
         <v>43657392451</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
+      <c r="A16" s="29" t="s">
         <v>66</v>
       </c>
-      <c r="B16">
+      <c r="B16" s="30">
         <v>10000</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="31">
         <v>44012</v>
       </c>
-      <c r="D16">
+      <c r="D16" s="32">
         <v>97535992218</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
+      <c r="A17" s="29" t="s">
         <v>67</v>
       </c>
-      <c r="B17">
+      <c r="B17" s="30">
         <v>7500</v>
       </c>
-      <c r="C17">
+      <c r="C17" s="31">
         <v>43667</v>
       </c>
-      <c r="D17">
+      <c r="D17" s="32">
         <v>79179596424</v>
       </c>
     </row>

</xml_diff>

<commit_message>
09 excel atalho alt
</commit_message>
<xml_diff>
--- a/004-atalhos/Atalhos-Use_Atalhos-Pasta_de_Trabalho1.xlsx
+++ b/004-atalhos/Atalhos-Use_Atalhos-Pasta_de_Trabalho1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jorge\Desktop\hashtag\hashtagExcel\004-atalhos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFF09E73-C943-466B-9C78-FB7D3A20D61E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84FDC29E-1993-461D-96DA-428AD074BCB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="978" activeTab="9" xr2:uid="{100ED8EA-C2B6-46A4-AE4B-962ED0DA143E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="978" activeTab="12" xr2:uid="{100ED8EA-C2B6-46A4-AE4B-962ED0DA143E}"/>
   </bookViews>
   <sheets>
     <sheet name="Ctrl T" sheetId="16" r:id="rId1"/>
@@ -326,7 +326,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -387,6 +387,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -415,7 +421,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -499,6 +505,12 @@
     <xf numFmtId="166" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -549,36 +561,6 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="pt-BR"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
@@ -601,13 +583,42 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent1">
+                    <a:satMod val="103000"/>
+                    <a:lumMod val="102000"/>
+                    <a:tint val="94000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent1">
+                    <a:satMod val="110000"/>
+                    <a:lumMod val="100000"/>
+                    <a:shade val="100000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="99000"/>
+                    <a:satMod val="120000"/>
+                    <a:shade val="78000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
             <a:ln>
               <a:noFill/>
             </a:ln>
-            <a:effectLst/>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
@@ -653,7 +664,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-A0AB-4F65-835A-9BDC8418D3CC}"/>
+              <c16:uniqueId val="{00000000-1104-494A-BD21-8BF66687E366}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -672,13 +683,42 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent2"/>
-            </a:solidFill>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent2">
+                    <a:satMod val="103000"/>
+                    <a:lumMod val="102000"/>
+                    <a:tint val="94000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent2">
+                    <a:satMod val="110000"/>
+                    <a:lumMod val="100000"/>
+                    <a:shade val="100000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent2">
+                    <a:lumMod val="99000"/>
+                    <a:satMod val="120000"/>
+                    <a:shade val="78000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
             <a:ln>
               <a:noFill/>
             </a:ln>
-            <a:effectLst/>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
@@ -724,7 +764,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-A0AB-4F65-835A-9BDC8418D3CC}"/>
+              <c16:uniqueId val="{00000001-1104-494A-BD21-8BF66687E366}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -743,13 +783,42 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent3"/>
-            </a:solidFill>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent3">
+                    <a:satMod val="103000"/>
+                    <a:lumMod val="102000"/>
+                    <a:tint val="94000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent3">
+                    <a:satMod val="110000"/>
+                    <a:lumMod val="100000"/>
+                    <a:shade val="100000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent3">
+                    <a:lumMod val="99000"/>
+                    <a:satMod val="120000"/>
+                    <a:shade val="78000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
             <a:ln>
               <a:noFill/>
             </a:ln>
-            <a:effectLst/>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
@@ -795,7 +864,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-A0AB-4F65-835A-9BDC8418D3CC}"/>
+              <c16:uniqueId val="{00000002-1104-494A-BD21-8BF66687E366}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -807,13 +876,12 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:gapWidth val="219"/>
-        <c:overlap val="-27"/>
-        <c:axId val="967414944"/>
-        <c:axId val="967400800"/>
+        <c:gapWidth val="100"/>
+        <c:axId val="724576048"/>
+        <c:axId val="724576528"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="967414944"/>
+        <c:axId val="724576048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -825,11 +893,11 @@
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="95000"/>
+                <a:alpha val="54000"/>
               </a:schemeClr>
             </a:solidFill>
             <a:round/>
@@ -843,9 +911,8 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
@@ -856,7 +923,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="967400800"/>
+        <c:crossAx val="724576528"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -864,7 +931,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="967400800"/>
+        <c:axId val="724576528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -874,9 +941,9 @@
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                  <a:alpha val="10000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:round/>
@@ -902,9 +969,8 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
@@ -915,7 +981,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="967414944"/>
+        <c:crossAx val="724576048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -928,7 +994,7 @@
       </c:spPr>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="b"/>
+      <c:legendPos val="t"/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -944,9 +1010,8 @@
           <a:pPr>
             <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="85000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
@@ -970,17 +1035,28 @@
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
+    <a:gradFill flip="none" rotWithShape="1">
+      <a:gsLst>
+        <a:gs pos="0">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:gs>
+        <a:gs pos="100000">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="85000"/>
+            <a:lumOff val="15000"/>
+          </a:schemeClr>
+        </a:gs>
+      </a:gsLst>
+      <a:path path="circle">
+        <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+      </a:path>
+      <a:tileRect/>
+    </a:gradFill>
+    <a:ln>
+      <a:noFill/>
     </a:ln>
     <a:effectLst/>
   </c:spPr>
@@ -996,7 +1072,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1043,35 +1119,33 @@
 </file>
 
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="209">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
+    <cs:defRPr sz="900" b="1" kern="1200" cap="all"/>
   </cs:axisTitle>
   <cs:categoryAxis>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -1079,26 +1153,34 @@
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+  <cs:chartArea>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
+      <a:gradFill flip="none" rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="65000"/>
+              <a:lumOff val="35000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="85000"/>
+              <a:lumOff val="15000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+        </a:path>
+        <a:tileRect/>
+      </a:gradFill>
     </cs:spPr>
     <cs:defRPr sz="1000" kern="1200"/>
   </cs:chartArea>
@@ -1107,9 +1189,8 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -1128,14 +1209,6 @@
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
     <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
@@ -1144,35 +1217,35 @@
   </cs:dataLabelCallout>
   <cs:dataPoint>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="3">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="0"/>
+    <cs:effectRef idx="3"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="3">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="0"/>
+    <cs:effectRef idx="3"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="28575" cap="rnd">
+      <a:ln w="34925" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -1184,30 +1257,31 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="3">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="0"/>
+    <cs:effectRef idx="3"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
   <cs:dataPointWireframe>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="rnd">
@@ -1223,21 +1297,18 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
@@ -1247,20 +1318,20 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
         </a:schemeClr>
       </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
       </a:ln>
@@ -1271,17 +1342,17 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
+        <a:prstDash val="dash"/>
       </a:ln>
     </cs:spPr>
   </cs:dropLine>
@@ -1290,14 +1361,13 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -1309,28 +1379,22 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
   </cs:floor>
   <cs:gridlineMajor>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="10000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -1342,17 +1406,16 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln>
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="5000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:gridlineMinor>
@@ -1361,17 +1424,17 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
+        <a:prstDash val="dash"/>
       </a:ln>
     </cs:spPr>
   </cs:hiLoLine>
@@ -1380,17 +1443,16 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:leaderLine>
@@ -1399,27 +1461,26 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+  <cs:plotArea>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
   </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+  <cs:plotArea3D>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
   </cs:plotArea3D>
   <cs:seriesAxis>
@@ -1427,11 +1488,21 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:seriesAxis>
   <cs:seriesLine>
@@ -1439,14 +1510,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -1458,12 +1529,19 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="95000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+    <cs:defRPr sz="1600" b="1" kern="1200" spc="100" baseline="0">
+      <a:effectLst>
+        <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="40000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:defRPr>
   </cs:title>
   <cs:trendline>
     <cs:lnRef idx="0">
@@ -1472,14 +1550,13 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="19050" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:prstDash val="sysDot"/>
       </a:ln>
     </cs:spPr>
   </cs:trendline>
@@ -1488,9 +1565,8 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -1500,7 +1576,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
@@ -1508,9 +1584,9 @@
       </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
       </a:ln>
@@ -1521,9 +1597,8 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -1533,14 +1608,8 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
   </cs:wall>
 </cs:chartStyle>
 </file>
@@ -1632,23 +1701,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>908050</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>50800</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1158875</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>53181</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>508000</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>31750</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>444500</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>129381</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Gráfico 1">
+        <xdr:cNvPr id="4" name="Chart 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{32D93B6C-2323-4D99-ABF5-48F68997834C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8ED24FD8-7028-BDCA-4981-4A1D7475B2CC}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4765,7 +4834,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86564475-C94C-4BAC-8A6A-7130AD288B94}">
   <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
@@ -5035,7 +5104,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13BA052D-BE13-48A5-B1F8-41D5A023B83E}">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection sqref="A1:D1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -5045,16 +5116,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="C1" s="34" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="20" t="s">
+      <c r="D1" s="34" t="s">
         <v>16</v>
       </c>
       <c r="E1" s="9"/>
@@ -17465,7 +17536,7 @@
         <v>13</v>
       </c>
       <c r="B6" s="21">
-        <f t="shared" ref="B6:D6" si="0">SUM(B2:B5)</f>
+        <f t="shared" ref="B6:C6" si="0">SUM(B2:B5)</f>
         <v>983653</v>
       </c>
       <c r="C6" s="21">

</xml_diff>

<commit_message>
10 atalhos excel fim
</commit_message>
<xml_diff>
--- a/004-atalhos/Atalhos-Use_Atalhos-Pasta_de_Trabalho1.xlsx
+++ b/004-atalhos/Atalhos-Use_Atalhos-Pasta_de_Trabalho1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jorge\Desktop\hashtag\hashtagExcel\004-atalhos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84FDC29E-1993-461D-96DA-428AD074BCB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7556A0F-2868-49D6-98DD-C0F666DFBAB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="978" activeTab="12" xr2:uid="{100ED8EA-C2B6-46A4-AE4B-962ED0DA143E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="978" activeTab="13" xr2:uid="{100ED8EA-C2B6-46A4-AE4B-962ED0DA143E}"/>
   </bookViews>
   <sheets>
     <sheet name="Ctrl T" sheetId="16" r:id="rId1"/>
@@ -71,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1449" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1463" uniqueCount="69">
   <si>
     <t>Vendedor</t>
   </si>
@@ -289,7 +289,7 @@
     <numFmt numFmtId="165" formatCode="&quot;R$&quot;\ #,##0.00"/>
     <numFmt numFmtId="166" formatCode="000&quot;.&quot;000&quot;.&quot;000&quot;-&quot;00"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -324,6 +324,14 @@
       <color theme="1"/>
       <name val="Abadi Extra Light"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="12">
@@ -418,10 +426,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -511,8 +520,11 @@
     <xf numFmtId="164" fontId="1" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="3">
@@ -5104,7 +5116,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13BA052D-BE13-48A5-B1F8-41D5A023B83E}">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
@@ -5201,7 +5213,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D25F7C08-0DA6-43FB-8459-A77277BAAA8F}">
   <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -5221,73 +5235,119 @@
       <c r="A2" t="s">
         <v>28</v>
       </c>
+      <c r="B2" s="35" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>19</v>
       </c>
+      <c r="B3" s="35" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
+      <c r="B4" s="35" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>12</v>
       </c>
+      <c r="B5" s="35" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>11</v>
       </c>
+      <c r="B6" s="35" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>21</v>
       </c>
+      <c r="B7" s="35" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>22</v>
       </c>
+      <c r="B8" s="35" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>20</v>
       </c>
+      <c r="B9" s="35" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>23</v>
       </c>
+      <c r="B10" s="35" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>24</v>
       </c>
+      <c r="B11" s="35" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>25</v>
       </c>
+      <c r="B12" s="35" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>26</v>
       </c>
+      <c r="B13" s="35" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>27</v>
       </c>
+      <c r="B14" s="36" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>51</v>
       </c>
+      <c r="B15" s="36" t="s">
+        <v>45</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B14" r:id="rId1" xr:uid="{D7E44D40-4DE3-4186-9427-AD2D9B1C4CBC}"/>
+    <hyperlink ref="B15" r:id="rId2" xr:uid="{711BD736-9E37-4A9C-9D3D-1FA1AF4ADF37}"/>
+  </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
aula 11 atalhos fim
</commit_message>
<xml_diff>
--- a/004-atalhos/Atalhos-Use_Atalhos-Pasta_de_Trabalho1.xlsx
+++ b/004-atalhos/Atalhos-Use_Atalhos-Pasta_de_Trabalho1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jorge\Desktop\hashtag\hashtagExcel\004-atalhos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7556A0F-2868-49D6-98DD-C0F666DFBAB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEDF93BF-3905-4205-9057-A5D24832D816}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="978" activeTab="13" xr2:uid="{100ED8EA-C2B6-46A4-AE4B-962ED0DA143E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="978" activeTab="15" xr2:uid="{100ED8EA-C2B6-46A4-AE4B-962ED0DA143E}"/>
   </bookViews>
   <sheets>
     <sheet name="Ctrl T" sheetId="16" r:id="rId1"/>
@@ -71,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1463" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1464" uniqueCount="70">
   <si>
     <t>Vendedor</t>
   </si>
@@ -217,9 +217,6 @@
     <t>Dia</t>
   </si>
   <si>
-    <t>Hota</t>
-  </si>
-  <si>
     <t>CPF</t>
   </si>
   <si>
@@ -278,6 +275,12 @@
   </si>
   <si>
     <t>Cachorro</t>
+  </si>
+  <si>
+    <t>Hora</t>
+  </si>
+  <si>
+    <t>Data Hora</t>
   </si>
 </sst>
 </file>
@@ -520,8 +523,8 @@
     <xf numFmtId="164" fontId="1" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -5213,7 +5216,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D25F7C08-0DA6-43FB-8459-A77277BAAA8F}">
   <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
@@ -5235,7 +5238,7 @@
       <c r="A2" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="35" t="s">
+      <c r="B2" t="s">
         <v>32</v>
       </c>
     </row>
@@ -5243,7 +5246,7 @@
       <c r="A3" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="35" t="s">
+      <c r="B3" t="s">
         <v>33</v>
       </c>
     </row>
@@ -5251,7 +5254,7 @@
       <c r="A4" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="35" t="s">
+      <c r="B4" t="s">
         <v>34</v>
       </c>
     </row>
@@ -5259,7 +5262,7 @@
       <c r="A5" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="35" t="s">
+      <c r="B5" t="s">
         <v>35</v>
       </c>
     </row>
@@ -5267,7 +5270,7 @@
       <c r="A6" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="35" t="s">
+      <c r="B6" t="s">
         <v>36</v>
       </c>
     </row>
@@ -5275,7 +5278,7 @@
       <c r="A7" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="35" t="s">
+      <c r="B7" t="s">
         <v>37</v>
       </c>
     </row>
@@ -5283,7 +5286,7 @@
       <c r="A8" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="35" t="s">
+      <c r="B8" t="s">
         <v>38</v>
       </c>
     </row>
@@ -5291,7 +5294,7 @@
       <c r="A9" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="35" t="s">
+      <c r="B9" t="s">
         <v>39</v>
       </c>
     </row>
@@ -5299,7 +5302,7 @@
       <c r="A10" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="35" t="s">
+      <c r="B10" t="s">
         <v>40</v>
       </c>
     </row>
@@ -5307,7 +5310,7 @@
       <c r="A11" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="35" t="s">
+      <c r="B11" t="s">
         <v>41</v>
       </c>
     </row>
@@ -5315,7 +5318,7 @@
       <c r="A12" t="s">
         <v>25</v>
       </c>
-      <c r="B12" s="35" t="s">
+      <c r="B12" t="s">
         <v>42</v>
       </c>
     </row>
@@ -5323,7 +5326,7 @@
       <c r="A13" t="s">
         <v>26</v>
       </c>
-      <c r="B13" s="35" t="s">
+      <c r="B13" t="s">
         <v>43</v>
       </c>
     </row>
@@ -5331,15 +5334,15 @@
       <c r="A14" t="s">
         <v>27</v>
       </c>
-      <c r="B14" s="36" t="s">
+      <c r="B14" s="35" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>51</v>
-      </c>
-      <c r="B15" s="36" t="s">
+        <v>50</v>
+      </c>
+      <c r="B15" s="35" t="s">
         <v>45</v>
       </c>
     </row>
@@ -5356,7 +5359,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22E6F5ED-CE74-4CE9-B1D0-6C7DE172826B}">
   <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11:XFD11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -5382,74 +5387,74 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="B3" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="27" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="27" t="s">
-        <v>34</v>
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="B5" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="B6" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>21</v>
-      </c>
-      <c r="B7" t="s">
-        <v>37</v>
+      <c r="A7" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="28" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>22</v>
-      </c>
-      <c r="B8" t="s">
-        <v>38</v>
+      <c r="A8" s="27" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="27" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="28" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B9" s="28" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="28" t="s">
-        <v>23</v>
-      </c>
-      <c r="B10" s="28" t="s">
-        <v>40</v>
+      <c r="A10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B11" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -5493,7 +5498,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9ED251FF-5AB3-4FE4-A8AF-1DF84087C6A3}">
   <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -5531,7 +5538,9 @@
       <c r="E2" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="F2" s="8"/>
+      <c r="F2" s="8">
+        <v>45115</v>
+      </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
@@ -5544,9 +5553,11 @@
         <v>4127</v>
       </c>
       <c r="E3" s="13" t="s">
-        <v>48</v>
-      </c>
-      <c r="F3" s="12"/>
+        <v>68</v>
+      </c>
+      <c r="F3" s="12">
+        <v>0.15902777777777777</v>
+      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
@@ -5557,6 +5568,12 @@
       </c>
       <c r="C4" s="2">
         <v>9603</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="F4" s="36">
+        <v>45115.160416666666</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -17199,7 +17216,7 @@
         <v>43987</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C17" s="2">
         <v>500</v>
@@ -17245,18 +17262,18 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="29" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B2" s="30">
         <v>10000</v>
@@ -17270,7 +17287,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="29" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B3" s="30">
         <v>3200</v>
@@ -17284,7 +17301,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="29" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B4" s="30">
         <v>7500</v>
@@ -17298,7 +17315,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="29" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B5" s="30">
         <v>10000</v>
@@ -17315,7 +17332,7 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="29" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B6" s="30">
         <v>3200</v>
@@ -17332,7 +17349,7 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="29" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B7" s="30">
         <v>10000</v>
@@ -17349,7 +17366,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="29" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B8" s="30">
         <v>3200</v>
@@ -17364,7 +17381,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="29" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B9" s="30">
         <v>7500</v>
@@ -17379,7 +17396,7 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="29" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B10" s="30">
         <v>3200</v>
@@ -17393,7 +17410,7 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="29" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B11" s="30">
         <v>10000</v>
@@ -17407,7 +17424,7 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="29" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B12" s="30">
         <v>10000</v>
@@ -17421,7 +17438,7 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="29" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B13" s="30">
         <v>3200</v>
@@ -17435,7 +17452,7 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="29" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B14" s="30">
         <v>7500</v>
@@ -17449,7 +17466,7 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="29" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B15" s="30">
         <v>7500</v>
@@ -17463,7 +17480,7 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="29" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B16" s="30">
         <v>10000</v>
@@ -17477,7 +17494,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="29" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B17" s="30">
         <v>7500</v>

</xml_diff>